<commit_message>
add excel field validation
</commit_message>
<xml_diff>
--- a/public/LoanDeposit/sample_loan_deposits.xlsx
+++ b/public/LoanDeposit/sample_loan_deposits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t xml:space="preserve">Branch Id</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">Created Date must be in Date Format as above Sample.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only One Sheet is Allowed. Otherwise Data cannot be Saved.</t>
   </si>
   <si>
     <t xml:space="preserve">Please Do See Sample Sheet give below</t>
@@ -244,7 +247,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,15 +264,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,11 +363,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.27"/>
   </cols>
@@ -437,10 +444,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -611,8 +618,13 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -627,14 +639,28 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A8:F8"/>
@@ -643,7 +669,7 @@
     <mergeCell ref="B11:N11"/>
     <mergeCell ref="B12:N12"/>
     <mergeCell ref="B13:N13"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -666,17 +692,17 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>10</v>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,7 +718,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,7 +734,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,7 +742,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +758,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,7 +766,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,7 +774,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -756,7 +782,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -764,7 +790,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +798,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -780,7 +806,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,7 +814,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,7 +822,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,7 +830,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,7 +846,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,7 +854,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,7 +862,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,7 +870,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,7 +878,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,7 +886,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,7 +894,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,7 +902,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,7 +910,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,7 +918,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>